<commit_message>
Add invoice example. Step 4.
</commit_message>
<xml_diff>
--- a/invoice.xlsx
+++ b/invoice.xlsx
@@ -320,7 +320,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true">
       <alignment indent="0" wrapText="false" textRotation="0" horizontal="center" vertical="center"/>
@@ -340,6 +340,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="14" xfId="0" applyBorder="true" applyFont="true" applyFill="true">
       <alignment indent="0" wrapText="false" textRotation="0"/>
@@ -533,53 +541,53 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="inlineStr">
+      <c r="A12" s="14" t="inlineStr">
         <is>
           <t>Always Good Computers</t>
         </is>
       </c>
-      <c r="B12" t="inlineStr">
+      <c r="B12" s="14" t="inlineStr">
         <is>
           <t>JerCo.</t>
         </is>
       </c>
-      <c r="C12" t="inlineStr">
+      <c r="C12" s="14" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
-      <c r="D12" t="inlineStr">
+      <c r="D12" s="14" t="inlineStr">
         <is>
           <t>Invoice Date:</t>
         </is>
       </c>
       <c r="E12" s="14" t="n">
-        <v>44366.0</v>
+        <v>44367.0</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="inlineStr">
+      <c r="A13" s="14" t="inlineStr">
         <is>
           <t>Joseph Lunar</t>
         </is>
       </c>
-      <c r="B13" t="inlineStr">
+      <c r="B13" s="14" t="inlineStr">
         <is>
           <t>Jeremy Corpse</t>
         </is>
       </c>
-      <c r="C13" t="inlineStr">
+      <c r="C13" s="14" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
-      <c r="D13" t="inlineStr">
+      <c r="D13" s="14" t="inlineStr">
         <is>
           <t>Due Date:</t>
         </is>
       </c>
       <c r="E13" s="14" t="n">
-        <v>44366.0</v>
+        <v>44367.0</v>
       </c>
     </row>
     <row r="14">
@@ -609,34 +617,34 @@
     <row r="16">
 </row>
     <row r="17">
-      <c r="A17" s="16" t="inlineStr">
+      <c r="A17" s="24" t="inlineStr">
         <is>
           <t>DESCRIPTION</t>
         </is>
       </c>
-      <c r="B17" s="16" t="inlineStr">
+      <c r="B17" s="24" t="inlineStr">
         <is>
           <t>QTY</t>
         </is>
       </c>
-      <c r="C17" s="16" t="inlineStr">
+      <c r="C17" s="24" t="inlineStr">
         <is>
           <t>UNIT PRICE</t>
         </is>
       </c>
-      <c r="D17" s="16" t="inlineStr">
+      <c r="D17" s="24" t="inlineStr">
         <is>
           <t>VAT</t>
         </is>
       </c>
-      <c r="E17" s="16" t="inlineStr">
+      <c r="E17" s="24" t="inlineStr">
         <is>
           <t>TOTAL</t>
         </is>
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="31" t="inlineStr">
+      <c r="A18" s="39" t="inlineStr">
         <is>
           <t>Laptop Acer</t>
         </is>
@@ -655,7 +663,7 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="31" t="inlineStr">
+      <c r="A19" s="39" t="inlineStr">
         <is>
           <t>Monitor Lenovo</t>
         </is>
@@ -674,7 +682,7 @@
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="31" t="inlineStr">
+      <c r="A20" s="39" t="inlineStr">
         <is>
           <t>Mechanical Keyboard Genesys</t>
         </is>
@@ -693,7 +701,7 @@
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="31" t="inlineStr">
+      <c r="A21" s="39" t="inlineStr">
         <is>
           <t>Mouse - Logitech M185</t>
         </is>
@@ -712,7 +720,7 @@
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="31" t="inlineStr">
+      <c r="A22" s="39" t="inlineStr">
         <is>
           <t>Headset - Syperlux HD330</t>
         </is>
@@ -731,7 +739,7 @@
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="31" t="inlineStr">
+      <c r="A23" s="39" t="inlineStr">
         <is>
           <t>IPhone 11</t>
         </is>
@@ -750,7 +758,7 @@
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="31" t="inlineStr">
+      <c r="A24" s="39" t="inlineStr">
         <is>
           <t>Desk</t>
         </is>
@@ -769,7 +777,7 @@
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="31" t="inlineStr">
+      <c r="A25" s="39" t="inlineStr">
         <is>
           <t>Mouse - Logitech M185</t>
         </is>
@@ -788,7 +796,7 @@
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="31" t="inlineStr">
+      <c r="A26" s="39" t="inlineStr">
         <is>
           <t>Mouse - Logitech M185</t>
         </is>
@@ -807,7 +815,7 @@
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="31" t="inlineStr">
+      <c r="A27" s="39" t="inlineStr">
         <is>
           <t>Mouse - Logitech M185</t>
         </is>
@@ -828,11 +836,9 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t/>
-        </is>
-      </c>
-      <c r="B28"/>
-      <c r="C28"/>
+          <t>Thank You for your business!</t>
+        </is>
+      </c>
       <c r="D28" t="inlineStr">
         <is>
           <t>Subtotal</t>
@@ -845,11 +851,9 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t/>
-        </is>
-      </c>
-      <c r="B29"/>
-      <c r="C29"/>
+          <t>Terms &amp; Instructions</t>
+        </is>
+      </c>
       <c r="D29" t="inlineStr">
         <is>
           <t>Discounts</t>
@@ -860,13 +864,6 @@
       </c>
     </row>
     <row r="30">
-      <c r="A30" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="B30"/>
-      <c r="C30"/>
       <c r="D30" t="inlineStr">
         <is>
           <t>Taxes</t>
@@ -877,13 +874,6 @@
       </c>
     </row>
     <row r="31">
-      <c r="A31" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="B31"/>
-      <c r="C31"/>
       <c r="D31" t="inlineStr">
         <is>
           <t>Total</t>
@@ -891,20 +881,6 @@
       </c>
       <c r="E31" t="n">
         <v>1935.5834</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="inlineStr">
-        <is>
-          <t>Thank You for your business!</t>
-        </is>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="inlineStr">
-        <is>
-          <t>Terms &amp; Instructions</t>
-        </is>
       </c>
     </row>
   </sheetData>
@@ -915,10 +891,6 @@
     <mergeCell ref="A3:C3"/>
     <mergeCell ref="A4:C4"/>
     <mergeCell ref="A5:C5"/>
-    <mergeCell ref="A28:C28"/>
-    <mergeCell ref="A29:C29"/>
-    <mergeCell ref="A30:C30"/>
-    <mergeCell ref="A31:C31"/>
   </mergeCells>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <drawing r:id="rId1"/>

</xml_diff>